<commit_message>
Global FLMA/B cal sheet and ingest corrections
added secondary controller engineering data stream, changed CTDMO depth
settings to 1450 and 5700, corrected reference designatros for recovered
CTDMO data.
</commit_message>
<xml_diff>
--- a/GA03FLMA/Omaha_Cal_Info_GA03FLMA_00001.xlsx
+++ b/GA03FLMA/Omaha_Cal_Info_GA03FLMA_00001.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Documents\Project Info\WHOI\Marine Integration - OOI\OOInet Migration\Integration\Cal and Ingest Sheets\Sheets from -test 2015-08-19\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="12720" windowHeight="12408"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -22,7 +17,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -959,7 +954,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -994,7 +989,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1205,26 +1200,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="4"/>
+    <col min="7" max="7" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="8" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -1262,7 +1257,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>73</v>
       </c>
@@ -1301,7 +1296,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="15" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
       <c r="D3" s="25"/>
       <c r="E3" s="26"/>
       <c r="F3" s="25"/>
@@ -1316,23 +1311,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="7" max="7" width="8.85546875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="11" customFormat="1" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1355,14 +1350,14 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>48</v>
       </c>
@@ -1388,7 +1383,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>48</v>
       </c>
@@ -1411,7 +1406,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>48</v>
       </c>
@@ -1431,7 +1426,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>48</v>
       </c>
@@ -1451,7 +1446,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>48</v>
       </c>
@@ -1471,7 +1466,7 @@
         <v>9.06E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>48</v>
       </c>
@@ -1491,7 +1486,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>48</v>
       </c>
@@ -1508,13 +1503,13 @@
         <v>43</v>
       </c>
       <c r="F9" s="2">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>48</v>
       </c>
@@ -1537,7 +1532,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>48</v>
       </c>
@@ -1554,13 +1549,13 @@
         <v>45</v>
       </c>
       <c r="F11" s="2">
-        <v>1.08</v>
+        <v>1.0760000000000001</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>48</v>
       </c>
@@ -1583,14 +1578,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>49</v>
       </c>
@@ -1616,7 +1611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>49</v>
       </c>
@@ -1636,7 +1631,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
         <v>49</v>
       </c>
@@ -1656,7 +1651,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>49</v>
       </c>
@@ -1676,7 +1671,7 @@
         <v>38502</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>49</v>
       </c>
@@ -1696,7 +1691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
         <v>49</v>
       </c>
@@ -1716,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
         <v>49</v>
       </c>
@@ -1739,14 +1734,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A21" s="21"/>
       <c r="B21" s="22"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
         <v>50</v>
       </c>
@@ -1772,7 +1767,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
         <v>50</v>
       </c>
@@ -1795,7 +1790,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
         <v>50</v>
       </c>
@@ -1815,14 +1810,14 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A25" s="21"/>
       <c r="B25" s="22"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
         <v>52</v>
       </c>
@@ -1848,7 +1843,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
         <v>52</v>
       </c>
@@ -1868,7 +1863,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
         <v>52</v>
       </c>
@@ -1888,7 +1883,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
         <v>52</v>
       </c>
@@ -1908,7 +1903,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A30" s="21" t="s">
         <v>52</v>
       </c>
@@ -1928,7 +1923,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
         <v>52</v>
       </c>
@@ -1948,7 +1943,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
         <v>52</v>
       </c>
@@ -1968,7 +1963,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>52</v>
       </c>
@@ -1988,7 +1983,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
         <v>52</v>
       </c>
@@ -2008,14 +2003,14 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A35" s="21"/>
       <c r="B35" s="22"/>
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
       <c r="E35" s="21"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
         <v>53</v>
       </c>
@@ -2032,7 +2027,7 @@
         <v>5</v>
       </c>
       <c r="F36" s="2">
-        <v>1000</v>
+        <v>1450</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>14</v>
@@ -2041,7 +2036,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>53</v>
       </c>
@@ -2061,7 +2056,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
         <v>53</v>
       </c>
@@ -2081,7 +2076,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>53</v>
       </c>
@@ -2101,14 +2096,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
       <c r="B40" s="22"/>
       <c r="C40" s="21"/>
       <c r="D40" s="21"/>
       <c r="E40" s="21"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>54</v>
       </c>
@@ -2125,7 +2120,7 @@
         <v>5</v>
       </c>
       <c r="F41" s="2">
-        <v>1000</v>
+        <v>1450</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>14</v>
@@ -2134,7 +2129,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>54</v>
       </c>
@@ -2154,7 +2149,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
         <v>54</v>
       </c>
@@ -2174,7 +2169,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
         <v>54</v>
       </c>
@@ -2194,14 +2189,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="21"/>
       <c r="B45" s="22"/>
       <c r="C45" s="21"/>
       <c r="D45" s="21"/>
       <c r="E45" s="21"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
         <v>55</v>
       </c>
@@ -2218,7 +2213,7 @@
         <v>5</v>
       </c>
       <c r="F46" s="2">
-        <v>1000</v>
+        <v>1450</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>14</v>
@@ -2227,7 +2222,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
         <v>55</v>
       </c>
@@ -2247,7 +2242,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
         <v>55</v>
       </c>
@@ -2267,7 +2262,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
         <v>55</v>
       </c>
@@ -2287,14 +2282,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
       <c r="B50" s="22"/>
       <c r="C50" s="21"/>
       <c r="D50" s="21"/>
       <c r="E50" s="21"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>56</v>
       </c>
@@ -2311,7 +2306,7 @@
         <v>5</v>
       </c>
       <c r="F51" s="2">
-        <v>1000</v>
+        <v>1450</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>14</v>
@@ -2320,7 +2315,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>56</v>
       </c>
@@ -2340,7 +2335,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>56</v>
       </c>
@@ -2360,7 +2355,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
         <v>56</v>
       </c>
@@ -2380,14 +2375,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
       <c r="B55" s="22"/>
       <c r="C55" s="21"/>
       <c r="D55" s="21"/>
       <c r="E55" s="21"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
         <v>57</v>
       </c>
@@ -2404,7 +2399,7 @@
         <v>5</v>
       </c>
       <c r="F56" s="2">
-        <v>1000</v>
+        <v>1450</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>14</v>
@@ -2413,7 +2408,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
         <v>57</v>
       </c>
@@ -2433,7 +2428,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
         <v>57</v>
       </c>
@@ -2453,7 +2448,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
         <v>57</v>
       </c>
@@ -2473,14 +2468,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
       <c r="B60" s="22"/>
       <c r="C60" s="21"/>
       <c r="D60" s="21"/>
       <c r="E60" s="21"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="21" t="s">
         <v>58</v>
       </c>
@@ -2497,7 +2492,7 @@
         <v>5</v>
       </c>
       <c r="F61" s="2">
-        <v>1000</v>
+        <v>1450</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>14</v>
@@ -2506,7 +2501,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="21" t="s">
         <v>58</v>
       </c>
@@ -2526,7 +2521,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
         <v>58</v>
       </c>
@@ -2546,7 +2541,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="21" t="s">
         <v>58</v>
       </c>
@@ -2566,14 +2561,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="21"/>
       <c r="B65" s="22"/>
       <c r="C65" s="21"/>
       <c r="D65" s="21"/>
       <c r="E65" s="21"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
         <v>59</v>
       </c>
@@ -2590,7 +2585,7 @@
         <v>5</v>
       </c>
       <c r="F66" s="2">
-        <v>1000</v>
+        <v>1450</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>14</v>
@@ -2599,7 +2594,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
         <v>59</v>
       </c>
@@ -2619,7 +2614,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
         <v>59</v>
       </c>
@@ -2639,7 +2634,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
         <v>59</v>
       </c>
@@ -2659,14 +2654,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="21"/>
       <c r="B70" s="22"/>
       <c r="C70" s="21"/>
       <c r="D70" s="21"/>
       <c r="E70" s="21"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="21" t="s">
         <v>60</v>
       </c>
@@ -2683,7 +2678,7 @@
         <v>5</v>
       </c>
       <c r="F71" s="2">
-        <v>1000</v>
+        <v>1450</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>14</v>
@@ -2692,7 +2687,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
         <v>60</v>
       </c>
@@ -2712,7 +2707,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="21" t="s">
         <v>60</v>
       </c>
@@ -2732,7 +2727,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="21" t="s">
         <v>60</v>
       </c>
@@ -2752,14 +2747,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="21"/>
       <c r="B75" s="22"/>
       <c r="C75" s="21"/>
       <c r="D75" s="21"/>
       <c r="E75" s="21"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
         <v>61</v>
       </c>
@@ -2776,7 +2771,7 @@
         <v>5</v>
       </c>
       <c r="F76" s="2">
-        <v>1000</v>
+        <v>1450</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>14</v>
@@ -2785,7 +2780,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="21" t="s">
         <v>61</v>
       </c>
@@ -2805,7 +2800,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="21" t="s">
         <v>61</v>
       </c>
@@ -2825,7 +2820,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="21" t="s">
         <v>61</v>
       </c>
@@ -2845,14 +2840,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="21"/>
       <c r="B80" s="22"/>
       <c r="C80" s="21"/>
       <c r="D80" s="21"/>
       <c r="E80" s="21"/>
     </row>
-    <row r="81" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
         <v>62</v>
       </c>
@@ -2869,7 +2864,7 @@
         <v>5</v>
       </c>
       <c r="F81" s="1">
-        <v>3500</v>
+        <v>5076</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>14</v>
@@ -2878,7 +2873,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="21" t="s">
         <v>62</v>
       </c>
@@ -2898,7 +2893,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="21" t="s">
         <v>62</v>
       </c>
@@ -2918,7 +2913,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="21" t="s">
         <v>62</v>
       </c>
@@ -2938,14 +2933,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="21"/>
       <c r="B85" s="22"/>
       <c r="C85" s="21"/>
       <c r="D85" s="21"/>
       <c r="E85" s="21"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="21" t="s">
         <v>63</v>
       </c>
@@ -2961,8 +2956,8 @@
       <c r="E86" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F86" s="2">
-        <v>3500</v>
+      <c r="F86" s="1">
+        <v>5076</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>14</v>
@@ -2971,7 +2966,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="21" t="s">
         <v>63</v>
       </c>
@@ -2991,7 +2986,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="21" t="s">
         <v>63</v>
       </c>
@@ -3011,7 +3006,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="21" t="s">
         <v>63</v>
       </c>
@@ -3031,14 +3026,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="21"/>
       <c r="B90" s="22"/>
       <c r="C90" s="21"/>
       <c r="D90" s="21"/>
       <c r="E90" s="21"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="21" t="s">
         <v>64</v>
       </c>
@@ -3054,8 +3049,8 @@
       <c r="E91" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F91" s="2">
-        <v>3500</v>
+      <c r="F91" s="1">
+        <v>5076</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>14</v>
@@ -3064,7 +3059,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="21" t="s">
         <v>64</v>
       </c>
@@ -3084,7 +3079,7 @@
         <v>-42.493000000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="21" t="s">
         <v>64</v>
       </c>
@@ -3104,7 +3099,7 @@
         <v>-42.962333333333333</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="21" t="s">
         <v>64</v>
       </c>
@@ -3124,14 +3119,14 @@
         <v>67</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="21"/>
       <c r="B95" s="22"/>
       <c r="C95" s="21"/>
       <c r="D95" s="21"/>
       <c r="E95" s="21"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="21" t="s">
         <v>65</v>
       </c>
@@ -3149,42 +3144,42 @@
         <v>72</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="21"/>
       <c r="B98" s="22"/>
       <c r="C98" s="21"/>
       <c r="D98" s="21"/>
       <c r="E98" s="21"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="21"/>
       <c r="B99" s="21"/>
       <c r="C99" s="21"/>
       <c r="D99" s="21"/>
       <c r="E99" s="21"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="21"/>
       <c r="B100" s="21"/>
       <c r="C100" s="21"/>
       <c r="D100" s="21"/>
       <c r="E100" s="21"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="21"/>
       <c r="D101" s="21"/>
       <c r="E101" s="21"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="21"/>
       <c r="B102" s="21"/>
       <c r="C102" s="21"/>
       <c r="D102" s="21"/>
       <c r="E102" s="21"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="21"/>
       <c r="B103" s="21"/>
       <c r="C103" s="21"/>

</xml_diff>

<commit_message>
Updates to Global FLanking Moorings ingest and cal sheets
Corrected Reference designators
Added inductive modem ID's
removed blank lines from Cal sheets
</commit_message>
<xml_diff>
--- a/GA03FLMA/Omaha_Cal_Info_GA03FLMA_00001.xlsx
+++ b/GA03FLMA/Omaha_Cal_Info_GA03FLMA_00001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12405" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -168,57 +168,12 @@
     <t>GA03FLMA-00001</t>
   </si>
   <si>
-    <t>GA03FLMA-RIS01-01-FLORTD000</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIS01-02-PHSENE000</t>
-  </si>
-  <si>
     <t>GA03FLMA-RIS01-03-DOSTAD000</t>
   </si>
   <si>
     <t>Requires TEMPWAT, PRESWAT, and PRACSAL from GA03FLMA-RIS02-03-CTDMOG000</t>
   </si>
   <si>
-    <t>GA03FLMA-RIS02-01-ADCPSL000</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIS02-03-CTDMOG000</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIS02-04-CTDMOG000</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIS02-05-CTDMOG000</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIS02-06-CTDMOG000</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIS02-07-CTDMOG000</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIS02-08-CTDMOG000</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIS02-09-CTDMOG000</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIS02-10-CTDMOG000</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIS02-11-CTDMOG000</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIS02-12-CTDMOH000</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIS02-13-CTDMOH000</t>
-  </si>
-  <si>
-    <t>GA03FLMA-RIS02-14-CTDMOH000</t>
-  </si>
-  <si>
     <t>GA03FLMA-FM001-00-ENG000000</t>
   </si>
   <si>
@@ -244,6 +199,51 @@
   </si>
   <si>
     <t>GA03FLMA</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIS01-05-FLORTD000</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-ADCPSL003</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG041</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG084</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG028</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG068</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG069</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG049</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG012</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG010</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOG096</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOH094</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOH018</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIM01-02-CTDMOH019</t>
+  </si>
+  <si>
+    <t>GA03FLMA-RIS01-04-PHSENF000</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="2" spans="1:13" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>47</v>
@@ -1275,16 +1275,16 @@
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="I2" s="3">
         <v>5165</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="18">
@@ -1309,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F91" sqref="F91"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1351,15 +1351,34 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="A2" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="21">
+        <v>1</v>
+      </c>
+      <c r="D2" s="21">
+        <v>1215</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="27">
+        <v>1.8700000000000001E-6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>47</v>
@@ -1371,21 +1390,18 @@
         <v>1215</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="27">
-        <v>1.8700000000000001E-6</v>
+        <v>10</v>
+      </c>
+      <c r="F3" s="2">
+        <v>51</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="2">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>47</v>
@@ -1397,18 +1413,15 @@
         <v>1215</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F4" s="2">
-        <v>51</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>40</v>
+        <v>1.21E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>47</v>
@@ -1420,15 +1433,15 @@
         <v>1215</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2">
-        <v>1.21E-2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>47</v>
@@ -1440,15 +1453,15 @@
         <v>1215</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F6" s="2">
-        <v>52</v>
+        <v>9.06E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>47</v>
@@ -1460,15 +1473,15 @@
         <v>1215</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2">
-        <v>9.06E-2</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>47</v>
@@ -1480,15 +1493,18 @@
         <v>1215</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="F8" s="2">
-        <v>45</v>
+        <v>124</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>47</v>
@@ -1500,10 +1516,10 @@
         <v>1215</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F9" s="2">
-        <v>124</v>
+        <v>700</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>42</v>
@@ -1511,7 +1527,7 @@
     </row>
     <row r="10" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>47</v>
@@ -1523,10 +1539,10 @@
         <v>1215</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F10" s="2">
-        <v>700</v>
+        <v>1.0760000000000001</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>42</v>
@@ -1534,7 +1550,7 @@
     </row>
     <row r="11" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>47</v>
@@ -1546,10 +1562,10 @@
         <v>1215</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F11" s="2">
-        <v>1.0760000000000001</v>
+        <v>3.9E-2</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>42</v>
@@ -1557,7 +1573,7 @@
     </row>
     <row r="12" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>47</v>
@@ -1565,29 +1581,45 @@
       <c r="C12" s="21">
         <v>1</v>
       </c>
-      <c r="D12" s="21">
-        <v>1215</v>
+      <c r="D12" s="21" t="s">
+        <v>54</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F12" s="2">
-        <v>3.9E-2</v>
+        <v>17533</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>42</v>
+        <v>14</v>
+      </c>
+      <c r="H12" s="2">
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="A13" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="21">
+        <v>1</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2229</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>47</v>
@@ -1596,24 +1628,18 @@
         <v>1</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F14" s="2">
-        <v>17533</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="2">
-        <v>29</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>47</v>
@@ -1622,18 +1648,18 @@
         <v>1</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F15" s="2">
-        <v>2229</v>
+        <v>38502</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>47</v>
@@ -1642,18 +1668,18 @@
         <v>1</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F16" s="2">
-        <v>101</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>47</v>
@@ -1662,18 +1688,18 @@
         <v>1</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F17" s="2">
-        <v>38502</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>47</v>
@@ -1682,18 +1708,21 @@
         <v>1</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F18" s="2">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>47</v>
@@ -1701,49 +1730,68 @@
       <c r="C19" s="21">
         <v>1</v>
       </c>
-      <c r="D19" s="21" t="s">
-        <v>69</v>
+      <c r="D19" s="21">
+        <v>428</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="F19" s="2">
-        <v>0</v>
+        <v>-42.493000000000002</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="2">
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="21">
+        <v>1</v>
+      </c>
+      <c r="D20" s="21">
+        <v>428</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="2">
+        <v>-42.962333333333333</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="21">
-        <v>1</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="2">
-        <v>35</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="21" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
+      <c r="A21" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="21">
+        <v>428</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B22" s="22" t="s">
         <v>47</v>
@@ -1752,7 +1800,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="21">
-        <v>428</v>
+        <v>20503</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>6</v>
@@ -1764,12 +1812,12 @@
         <v>14</v>
       </c>
       <c r="H22" s="2">
-        <v>29</v>
+        <v>500</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B23" s="22" t="s">
         <v>47</v>
@@ -1778,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="21">
-        <v>428</v>
+        <v>20503</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>7</v>
@@ -1786,13 +1834,10 @@
       <c r="F23" s="2">
         <v>-42.962333333333333</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="24" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>47</v>
@@ -1801,25 +1846,38 @@
         <v>1</v>
       </c>
       <c r="D24" s="21">
-        <v>428</v>
+        <v>20503</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>71</v>
+        <v>8</v>
+      </c>
+      <c r="F24" s="2">
+        <v>-42.493000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="A25" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="21">
+        <v>1</v>
+      </c>
+      <c r="D25" s="21">
+        <v>20503</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="2">
+        <v>-42.962333333333333</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B26" s="22" t="s">
         <v>47</v>
@@ -1831,21 +1889,15 @@
         <v>20503</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>-42.493000000000002</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="2">
-        <v>500</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B27" s="22" t="s">
         <v>47</v>
@@ -1857,15 +1909,15 @@
         <v>20503</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F27" s="2">
-        <v>-42.962333333333333</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B28" s="22" t="s">
         <v>47</v>
@@ -1877,15 +1929,15 @@
         <v>20503</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F28" s="2">
-        <v>-42.493000000000002</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B29" s="22" t="s">
         <v>47</v>
@@ -1897,15 +1949,15 @@
         <v>20503</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F29" s="2">
-        <v>-42.962333333333333</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A30" s="21" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>47</v>
@@ -1917,15 +1969,15 @@
         <v>20503</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F30" s="2">
-        <v>500000</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>47</v>
@@ -1934,18 +1986,24 @@
         <v>1</v>
       </c>
       <c r="D31" s="21">
-        <v>20503</v>
+        <v>12401</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F31" s="2">
-        <v>0.45</v>
+        <v>1450</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="2">
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B32" s="22" t="s">
         <v>47</v>
@@ -1954,18 +2012,18 @@
         <v>1</v>
       </c>
       <c r="D32" s="21">
-        <v>20503</v>
+        <v>12401</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="F32" s="2">
-        <v>0.45</v>
+        <v>-42.493000000000002</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>47</v>
@@ -1974,18 +2032,18 @@
         <v>1</v>
       </c>
       <c r="D33" s="21">
-        <v>20503</v>
+        <v>12401</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="F33" s="2">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
+        <v>-42.962333333333333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B34" s="22" t="s">
         <v>47</v>
@@ -1994,25 +2052,44 @@
         <v>1</v>
       </c>
       <c r="D34" s="21">
-        <v>20503</v>
+        <v>12401</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F34" s="2">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-    </row>
-    <row r="36" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1</v>
+      </c>
+      <c r="D35" s="21">
+        <v>12396</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1450</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B36" s="22" t="s">
         <v>47</v>
@@ -2021,64 +2098,58 @@
         <v>1</v>
       </c>
       <c r="D36" s="21">
-        <v>12401</v>
+        <v>12396</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F36" s="2">
-        <v>1450</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="2">
+        <v>-42.493000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="21">
+        <v>1</v>
+      </c>
+      <c r="D37" s="21">
+        <v>12396</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="2">
+        <v>-42.962333333333333</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="21">
+        <v>1</v>
+      </c>
+      <c r="D38" s="21">
+        <v>12396</v>
+      </c>
+      <c r="E38" s="21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A37" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="21">
-        <v>1</v>
-      </c>
-      <c r="D37" s="21">
-        <v>12401</v>
-      </c>
-      <c r="E37" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F37" s="2">
-        <v>-42.493000000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A38" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="21">
-        <v>1</v>
-      </c>
-      <c r="D38" s="21">
-        <v>12401</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>7</v>
-      </c>
       <c r="F38" s="2">
-        <v>-42.962333333333333</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B39" s="22" t="s">
         <v>47</v>
@@ -2087,25 +2158,44 @@
         <v>1</v>
       </c>
       <c r="D39" s="21">
-        <v>12401</v>
+        <v>12584</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="F39" s="2">
-        <v>57</v>
+        <v>1450</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="2">
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
+      <c r="A40" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="21">
+        <v>1</v>
+      </c>
+      <c r="D40" s="21">
+        <v>12584</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="2">
+        <v>-42.493000000000002</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>47</v>
@@ -2114,24 +2204,18 @@
         <v>1</v>
       </c>
       <c r="D41" s="21">
-        <v>12396</v>
+        <v>12584</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F41" s="2">
-        <v>1450</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H41" s="2">
-        <v>39</v>
+        <v>-42.962333333333333</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B42" s="22" t="s">
         <v>47</v>
@@ -2140,18 +2224,18 @@
         <v>1</v>
       </c>
       <c r="D42" s="21">
-        <v>12396</v>
+        <v>12584</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="F42" s="2">
-        <v>-42.493000000000002</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B43" s="22" t="s">
         <v>47</v>
@@ -2160,18 +2244,24 @@
         <v>1</v>
       </c>
       <c r="D43" s="21">
-        <v>12396</v>
+        <v>12408</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F43" s="2">
-        <v>-42.962333333333333</v>
+        <v>1450</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" s="2">
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B44" s="22" t="s">
         <v>47</v>
@@ -2180,25 +2270,38 @@
         <v>1</v>
       </c>
       <c r="D44" s="21">
-        <v>12396</v>
+        <v>12408</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="F44" s="2">
-        <v>20</v>
+        <v>-42.493000000000002</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="21"/>
-      <c r="B45" s="22"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
+      <c r="A45" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="21">
+        <v>1</v>
+      </c>
+      <c r="D45" s="21">
+        <v>12408</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="2">
+        <v>-42.962333333333333</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B46" s="22" t="s">
         <v>47</v>
@@ -2207,24 +2310,18 @@
         <v>1</v>
       </c>
       <c r="D46" s="21">
-        <v>12584</v>
+        <v>12408</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="F46" s="2">
-        <v>1450</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H46" s="2">
-        <v>59</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B47" s="22" t="s">
         <v>47</v>
@@ -2233,18 +2330,24 @@
         <v>1</v>
       </c>
       <c r="D47" s="21">
-        <v>12584</v>
+        <v>12608</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" s="2">
-        <v>-42.493000000000002</v>
+        <v>1450</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="2">
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B48" s="22" t="s">
         <v>47</v>
@@ -2253,18 +2356,18 @@
         <v>1</v>
       </c>
       <c r="D48" s="21">
-        <v>12584</v>
+        <v>12608</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.493000000000002</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B49" s="22" t="s">
         <v>47</v>
@@ -2273,25 +2376,38 @@
         <v>1</v>
       </c>
       <c r="D49" s="21">
-        <v>12584</v>
+        <v>12608</v>
       </c>
       <c r="E49" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="2">
+        <v>-42.962333333333333</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="21">
+        <v>1</v>
+      </c>
+      <c r="D50" s="21">
+        <v>12608</v>
+      </c>
+      <c r="E50" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F49" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="21"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
+      <c r="F50" s="2">
+        <v>54</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B51" s="22" t="s">
         <v>47</v>
@@ -2300,7 +2416,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="21">
-        <v>12408</v>
+        <v>12609</v>
       </c>
       <c r="E51" s="21" t="s">
         <v>5</v>
@@ -2312,12 +2428,12 @@
         <v>14</v>
       </c>
       <c r="H51" s="2">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B52" s="22" t="s">
         <v>47</v>
@@ -2326,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="D52" s="21">
-        <v>12408</v>
+        <v>12609</v>
       </c>
       <c r="E52" s="21" t="s">
         <v>6</v>
@@ -2337,7 +2453,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B53" s="22" t="s">
         <v>47</v>
@@ -2346,7 +2462,7 @@
         <v>1</v>
       </c>
       <c r="D53" s="21">
-        <v>12408</v>
+        <v>12609</v>
       </c>
       <c r="E53" s="21" t="s">
         <v>7</v>
@@ -2357,7 +2473,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B54" s="22" t="s">
         <v>47</v>
@@ -2366,25 +2482,44 @@
         <v>1</v>
       </c>
       <c r="D54" s="21">
-        <v>12408</v>
+        <v>12609</v>
       </c>
       <c r="E54" s="21" t="s">
         <v>29</v>
       </c>
       <c r="F54" s="2">
-        <v>15</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="21"/>
-      <c r="B55" s="22"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
+      <c r="A55" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" s="21">
+        <v>1</v>
+      </c>
+      <c r="D55" s="21">
+        <v>12409</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1450</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H55" s="2">
+        <v>250</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B56" s="22" t="s">
         <v>47</v>
@@ -2393,24 +2528,18 @@
         <v>1</v>
       </c>
       <c r="D56" s="21">
-        <v>12608</v>
+        <v>12409</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F56" s="2">
-        <v>1450</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H56" s="2">
-        <v>130</v>
+        <v>-42.493000000000002</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B57" s="22" t="s">
         <v>47</v>
@@ -2419,18 +2548,18 @@
         <v>1</v>
       </c>
       <c r="D57" s="21">
-        <v>12608</v>
+        <v>12409</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F57" s="2">
-        <v>-42.493000000000002</v>
+        <v>-42.962333333333333</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B58" s="22" t="s">
         <v>47</v>
@@ -2439,18 +2568,18 @@
         <v>1</v>
       </c>
       <c r="D58" s="21">
-        <v>12608</v>
+        <v>12409</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F58" s="2">
-        <v>-42.962333333333333</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B59" s="22" t="s">
         <v>47</v>
@@ -2459,25 +2588,44 @@
         <v>1</v>
       </c>
       <c r="D59" s="21">
-        <v>12608</v>
+        <v>12412</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="F59" s="2">
-        <v>54</v>
+        <v>1450</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H59" s="2">
+        <v>350</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="21"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
+      <c r="A60" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" s="21">
+        <v>1</v>
+      </c>
+      <c r="D60" s="21">
+        <v>12412</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" s="2">
+        <v>-42.493000000000002</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="21" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B61" s="22" t="s">
         <v>47</v>
@@ -2486,24 +2634,18 @@
         <v>1</v>
       </c>
       <c r="D61" s="21">
-        <v>12609</v>
+        <v>12412</v>
       </c>
       <c r="E61" s="21" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F61" s="2">
-        <v>1450</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H61" s="2">
-        <v>180</v>
+        <v>-42.962333333333333</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="21" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B62" s="22" t="s">
         <v>47</v>
@@ -2512,18 +2654,18 @@
         <v>1</v>
       </c>
       <c r="D62" s="21">
-        <v>12609</v>
+        <v>12412</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="F62" s="2">
-        <v>-42.493000000000002</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B63" s="22" t="s">
         <v>47</v>
@@ -2532,18 +2674,24 @@
         <v>1</v>
       </c>
       <c r="D63" s="21">
-        <v>12609</v>
+        <v>12410</v>
       </c>
       <c r="E63" s="21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F63" s="2">
-        <v>-42.962333333333333</v>
+        <v>1450</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H63" s="2">
+        <v>501</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="21" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B64" s="22" t="s">
         <v>47</v>
@@ -2552,25 +2700,38 @@
         <v>1</v>
       </c>
       <c r="D64" s="21">
-        <v>12609</v>
+        <v>12410</v>
       </c>
       <c r="E64" s="21" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="F64" s="2">
-        <v>62</v>
+        <v>-42.493000000000002</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="21"/>
-      <c r="B65" s="22"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="21"/>
+      <c r="A65" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C65" s="21">
+        <v>1</v>
+      </c>
+      <c r="D65" s="21">
+        <v>12410</v>
+      </c>
+      <c r="E65" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="2">
+        <v>-42.962333333333333</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B66" s="22" t="s">
         <v>47</v>
@@ -2579,44 +2740,44 @@
         <v>1</v>
       </c>
       <c r="D66" s="21">
-        <v>12409</v>
+        <v>12410</v>
       </c>
       <c r="E66" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F66" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C67" s="24">
+        <v>1</v>
+      </c>
+      <c r="D67" s="24">
+        <v>12394</v>
+      </c>
+      <c r="E67" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F66" s="2">
-        <v>1450</v>
-      </c>
-      <c r="G66" s="2" t="s">
+      <c r="F67" s="1">
+        <v>5076</v>
+      </c>
+      <c r="G67" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H66" s="2">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B67" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C67" s="21">
-        <v>1</v>
-      </c>
-      <c r="D67" s="21">
-        <v>12409</v>
-      </c>
-      <c r="E67" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F67" s="2">
-        <v>-42.493000000000002</v>
+      <c r="H67" s="1">
+        <v>748</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B68" s="22" t="s">
         <v>47</v>
@@ -2625,18 +2786,18 @@
         <v>1</v>
       </c>
       <c r="D68" s="21">
-        <v>12409</v>
+        <v>12394</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" s="2">
-        <v>-42.962333333333333</v>
+        <v>-42.493000000000002</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B69" s="22" t="s">
         <v>47</v>
@@ -2645,25 +2806,38 @@
         <v>1</v>
       </c>
       <c r="D69" s="21">
-        <v>12409</v>
+        <v>12394</v>
       </c>
       <c r="E69" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="2">
+        <v>-42.962333333333333</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C70" s="21">
+        <v>1</v>
+      </c>
+      <c r="D70" s="21">
+        <v>12394</v>
+      </c>
+      <c r="E70" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F69" s="2">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="21"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
-      <c r="E70" s="21"/>
+      <c r="F70" s="2">
+        <v>26</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="21" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B71" s="22" t="s">
         <v>47</v>
@@ -2672,24 +2846,24 @@
         <v>1</v>
       </c>
       <c r="D71" s="21">
-        <v>12412</v>
+        <v>12618</v>
       </c>
       <c r="E71" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F71" s="2">
-        <v>1450</v>
+      <c r="F71" s="1">
+        <v>5076</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H71" s="2">
-        <v>350</v>
+        <v>999</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B72" s="22" t="s">
         <v>47</v>
@@ -2698,7 +2872,7 @@
         <v>1</v>
       </c>
       <c r="D72" s="21">
-        <v>12412</v>
+        <v>12618</v>
       </c>
       <c r="E72" s="21" t="s">
         <v>6</v>
@@ -2709,7 +2883,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="21" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B73" s="22" t="s">
         <v>47</v>
@@ -2718,7 +2892,7 @@
         <v>1</v>
       </c>
       <c r="D73" s="21">
-        <v>12412</v>
+        <v>12618</v>
       </c>
       <c r="E73" s="21" t="s">
         <v>7</v>
@@ -2729,7 +2903,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="21" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B74" s="22" t="s">
         <v>47</v>
@@ -2738,25 +2912,44 @@
         <v>1</v>
       </c>
       <c r="D74" s="21">
-        <v>12412</v>
+        <v>12618</v>
       </c>
       <c r="E74" s="21" t="s">
         <v>29</v>
       </c>
       <c r="F74" s="2">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="21"/>
-      <c r="B75" s="22"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
-      <c r="E75" s="21"/>
+      <c r="A75" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C75" s="21">
+        <v>1</v>
+      </c>
+      <c r="D75" s="21">
+        <v>12619</v>
+      </c>
+      <c r="E75" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F75" s="1">
+        <v>5076</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H75" s="2">
+        <v>1501</v>
+      </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B76" s="22" t="s">
         <v>47</v>
@@ -2765,24 +2958,18 @@
         <v>1</v>
       </c>
       <c r="D76" s="21">
-        <v>12410</v>
+        <v>12619</v>
       </c>
       <c r="E76" s="21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F76" s="2">
-        <v>1450</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H76" s="2">
-        <v>501</v>
+        <v>-42.493000000000002</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="21" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B77" s="22" t="s">
         <v>47</v>
@@ -2791,18 +2978,18 @@
         <v>1</v>
       </c>
       <c r="D77" s="21">
-        <v>12410</v>
+        <v>12619</v>
       </c>
       <c r="E77" s="21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F77" s="2">
-        <v>-42.493000000000002</v>
+        <v>-42.962333333333333</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="21" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B78" s="22" t="s">
         <v>47</v>
@@ -2811,18 +2998,18 @@
         <v>1</v>
       </c>
       <c r="D78" s="21">
-        <v>12410</v>
+        <v>12619</v>
       </c>
       <c r="E78" s="21" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F78" s="2">
-        <v>-42.962333333333333</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B79" s="22" t="s">
         <v>47</v>
@@ -2830,361 +3017,55 @@
       <c r="C79" s="21">
         <v>1</v>
       </c>
-      <c r="D79" s="21">
-        <v>12410</v>
-      </c>
-      <c r="E79" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F79" s="2">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="21"/>
-      <c r="B80" s="22"/>
-      <c r="C80" s="21"/>
-      <c r="D80" s="21"/>
-      <c r="E80" s="21"/>
-    </row>
-    <row r="81" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B81" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C81" s="24">
-        <v>1</v>
-      </c>
-      <c r="D81" s="24">
-        <v>12394</v>
-      </c>
-      <c r="E81" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="F81" s="1">
-        <v>5076</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H81" s="1">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B82" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C82" s="21">
-        <v>1</v>
-      </c>
-      <c r="D82" s="21">
-        <v>12394</v>
-      </c>
-      <c r="E82" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F82" s="2">
-        <v>-42.493000000000002</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B83" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C83" s="21">
-        <v>1</v>
-      </c>
-      <c r="D83" s="21">
-        <v>12394</v>
-      </c>
-      <c r="E83" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F83" s="2">
-        <v>-42.962333333333333</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B84" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C84" s="21">
-        <v>1</v>
-      </c>
-      <c r="D84" s="21">
-        <v>12394</v>
-      </c>
-      <c r="E84" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F84" s="2">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D79" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E79" s="21"/>
+      <c r="G79" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="21"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="21"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="21"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="21"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="21"/>
+      <c r="B83" s="21"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="21"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="21"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="21"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="21"/>
-      <c r="B85" s="22"/>
+      <c r="B85" s="21"/>
       <c r="C85" s="21"/>
       <c r="D85" s="21"/>
       <c r="E85" s="21"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B86" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C86" s="21">
-        <v>1</v>
-      </c>
-      <c r="D86" s="21">
-        <v>12618</v>
-      </c>
-      <c r="E86" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="F86" s="1">
-        <v>5076</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H86" s="2">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B87" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C87" s="21">
-        <v>1</v>
-      </c>
-      <c r="D87" s="21">
-        <v>12618</v>
-      </c>
-      <c r="E87" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F87" s="2">
-        <v>-42.493000000000002</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B88" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C88" s="21">
-        <v>1</v>
-      </c>
-      <c r="D88" s="21">
-        <v>12618</v>
-      </c>
-      <c r="E88" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F88" s="2">
-        <v>-42.962333333333333</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B89" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C89" s="21">
-        <v>1</v>
-      </c>
-      <c r="D89" s="21">
-        <v>12618</v>
-      </c>
-      <c r="E89" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F89" s="2">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="21"/>
-      <c r="B90" s="22"/>
-      <c r="C90" s="21"/>
-      <c r="D90" s="21"/>
-      <c r="E90" s="21"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B91" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C91" s="21">
-        <v>1</v>
-      </c>
-      <c r="D91" s="21">
-        <v>12619</v>
-      </c>
-      <c r="E91" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="F91" s="1">
-        <v>5076</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H91" s="2">
-        <v>1501</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B92" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C92" s="21">
-        <v>1</v>
-      </c>
-      <c r="D92" s="21">
-        <v>12619</v>
-      </c>
-      <c r="E92" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F92" s="2">
-        <v>-42.493000000000002</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B93" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C93" s="21">
-        <v>1</v>
-      </c>
-      <c r="D93" s="21">
-        <v>12619</v>
-      </c>
-      <c r="E93" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F93" s="2">
-        <v>-42.962333333333333</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B94" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C94" s="21">
-        <v>1</v>
-      </c>
-      <c r="D94" s="21">
-        <v>12619</v>
-      </c>
-      <c r="E94" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F94" s="2">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="21"/>
-      <c r="B95" s="22"/>
-      <c r="C95" s="21"/>
-      <c r="D95" s="21"/>
-      <c r="E95" s="21"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B96" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C96" s="21">
-        <v>1</v>
-      </c>
-      <c r="D96" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E96" s="21"/>
-      <c r="G96" s="28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="21"/>
-      <c r="B98" s="22"/>
-      <c r="C98" s="21"/>
-      <c r="D98" s="21"/>
-      <c r="E98" s="21"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="21"/>
-      <c r="B99" s="21"/>
-      <c r="C99" s="21"/>
-      <c r="D99" s="21"/>
-      <c r="E99" s="21"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="21"/>
-      <c r="B100" s="21"/>
-      <c r="C100" s="21"/>
-      <c r="D100" s="21"/>
-      <c r="E100" s="21"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="21"/>
-      <c r="B101" s="21"/>
-      <c r="C101" s="21"/>
-      <c r="D101" s="21"/>
-      <c r="E101" s="21"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="21"/>
-      <c r="B102" s="21"/>
-      <c r="C102" s="21"/>
-      <c r="D102" s="21"/>
-      <c r="E102" s="21"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="21"/>
-      <c r="B103" s="21"/>
-      <c r="C103" s="21"/>
-      <c r="D103" s="21"/>
-      <c r="E103" s="21"/>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="21"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>